<commit_message>
consolidate data from .log files
</commit_message>
<xml_diff>
--- a/english_auction_data.xlsx
+++ b/english_auction_data.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CS\LLMauctions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DF53C96-55EE-465A-8814-9DD1CEFFBF2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{148D0A6C-D38F-42AB-AF92-6E1F4D7633E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{02E901B6-7723-420C-9BF2-7026BA83D7F3}"/>
+    <workbookView xWindow="9204" yWindow="0" windowWidth="13932" windowHeight="12336" activeTab="3" xr2:uid="{02E901B6-7723-420C-9BF2-7026BA83D7F3}"/>
   </bookViews>
   <sheets>
     <sheet name="3.5 Sonnet" sheetId="1" r:id="rId1"/>
     <sheet name="4o" sheetId="2" r:id="rId2"/>
     <sheet name="4o-mini" sheetId="3" r:id="rId3"/>
+    <sheet name="gemini-pro" sheetId="4" r:id="rId4"/>
+    <sheet name="gemini-flash" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="18">
   <si>
     <t>Round 0</t>
   </si>
@@ -80,6 +82,18 @@
   </si>
   <si>
     <t>Paid</t>
+  </si>
+  <si>
+    <t>Everyone bids 2</t>
+  </si>
+  <si>
+    <t>avg</t>
+  </si>
+  <si>
+    <t>median</t>
+  </si>
+  <si>
+    <t>std.dev</t>
   </si>
 </sst>
 </file>
@@ -457,15 +471,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B74CD0F-D9A9-41F2-8A12-86D1C35A3BC4}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14:D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>12</v>
       </c>
@@ -473,7 +487,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -484,7 +498,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -495,7 +509,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -506,7 +520,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -517,7 +531,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -528,7 +542,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -539,7 +553,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -550,7 +564,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -561,7 +575,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -572,7 +586,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -583,7 +597,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -594,7 +608,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -603,6 +617,24 @@
       </c>
       <c r="C13">
         <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D14">
+        <f>AVERAGE(C2:C13)</f>
+        <v>36.75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D15">
+        <f>MEDIAN(C2:C13)</f>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D16">
+        <f>_xlfn.STDEV.S(C2:C13)</f>
+        <v>1.6025547785276542</v>
       </c>
     </row>
   </sheetData>
@@ -613,15 +645,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{106EB011-AE23-49AE-9A91-A4C3EAF792B6}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C1"/>
+      <selection activeCell="D13" sqref="D13:D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>12</v>
       </c>
@@ -629,7 +661,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -640,7 +672,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -651,7 +683,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -662,7 +694,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -673,7 +705,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -684,7 +716,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -695,7 +727,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -706,7 +738,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -717,7 +749,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -728,7 +760,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -739,7 +771,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -748,6 +780,24 @@
       </c>
       <c r="C12">
         <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D13">
+        <f>AVERAGE(C1:C12)</f>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D14">
+        <f>MEDIAN(C1:C12)</f>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D15">
+        <f>_xlfn.STDEV.S(C1:C12)</f>
+        <v>0.89442719099991586</v>
       </c>
     </row>
   </sheetData>
@@ -757,15 +807,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{090321E5-1425-4018-B019-BD0293D7D0CC}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C1"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>12</v>
       </c>
@@ -773,7 +823,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -784,7 +834,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -795,7 +845,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -806,7 +856,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -817,7 +867,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -828,7 +878,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -839,7 +889,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -850,7 +900,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -861,7 +911,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -872,7 +922,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -883,7 +933,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -892,9 +942,294 @@
       </c>
       <c r="C12">
         <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D13">
+        <f>AVERAGE(C1:C12)</f>
+        <v>3.2727272727272729</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D14">
+        <f>MEDIAN(C1:C12)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D15">
+        <f>_xlfn.STDEV.S(C1:C12)</f>
+        <v>0.46709936649691436</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4E70412-0567-4212-BF4B-7F64A7C06704}">
+  <dimension ref="A2:D15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>8</v>
+      </c>
+      <c r="C2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>8</v>
+      </c>
+      <c r="C8">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>8</v>
+      </c>
+      <c r="C11">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>8</v>
+      </c>
+      <c r="C12">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13">
+        <f>AVERAGE(C1:C12)</f>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14">
+        <f>MEDIAN(C1:C12)</f>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15">
+        <f>_xlfn.STDEV.S(C1:C12)</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5380F8FD-6522-4E6D-AF61-C648BD6C8F63}">
+  <dimension ref="A2:B12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>